<commit_message>
fixed excel total absences
</commit_message>
<xml_diff>
--- a/exceltocsv/public/reports/employee_dtr/Arceo,Arwin.xlsx
+++ b/exceltocsv/public/reports/employee_dtr/Arceo,Arwin.xlsx
@@ -9,7 +9,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="64" xml:space="preserve">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="68" xml:space="preserve">
   <si>
     <t>iRipple, Inc.</t>
   </si>
@@ -68,85 +68,94 @@
     <t>REMARKS</t>
   </si>
   <si>
-    <t>03-21-2015</t>
+    <t>05-09-2015</t>
   </si>
   <si>
     <t>Saturday</t>
   </si>
   <si>
-    <t>08:30:00</t>
-  </si>
-  <si>
-    <t>18:30:00</t>
-  </si>
-  <si>
-    <t>~OB Others|Mydin live integration for all Branches.|</t>
-  </si>
-  <si>
-    <t>03-22-2015</t>
+    <t>05-10-2015</t>
   </si>
   <si>
     <t>Sunday</t>
   </si>
   <si>
-    <t>03-23-2015</t>
+    <t>05-11-2015</t>
   </si>
   <si>
     <t>Monday</t>
   </si>
   <si>
-    <t>03-24-2015</t>
+    <t>05-12-2015</t>
   </si>
   <si>
     <t>Tuesday</t>
   </si>
   <si>
-    <t>03-25-2015</t>
+    <t>05-13-2015</t>
   </si>
   <si>
     <t>Wednesday</t>
   </si>
   <si>
-    <t>03-26-2015</t>
+    <t>05-14-2015</t>
   </si>
   <si>
     <t>Thursday</t>
   </si>
   <si>
-    <t>03-27-2015</t>
+    <t>05-15-2015</t>
   </si>
   <si>
     <t>Friday</t>
   </si>
   <si>
-    <t>03-28-2015</t>
-  </si>
-  <si>
-    <t>03-29-2015</t>
-  </si>
-  <si>
-    <t>03-30-2015</t>
-  </si>
-  <si>
-    <t>03-31-2015</t>
-  </si>
-  <si>
-    <t>04-01-2015</t>
-  </si>
-  <si>
-    <t>~VL Rest and vacation with my family.</t>
-  </si>
-  <si>
-    <t>04-02-2015</t>
-  </si>
-  <si>
-    <t>~Special Day - Maundy Thursday ( Regular Holiday )</t>
-  </si>
-  <si>
-    <t>04-03-2015</t>
-  </si>
-  <si>
-    <t>~Special Day - Good Friday ( Regular Holiday )</t>
+    <t>05-16-2015</t>
+  </si>
+  <si>
+    <t>05-17-2015</t>
+  </si>
+  <si>
+    <t>05-18-2015</t>
+  </si>
+  <si>
+    <t>~VL Need to go with my son for his ear check up</t>
+  </si>
+  <si>
+    <t>05-19-2015</t>
+  </si>
+  <si>
+    <t>07:21:41</t>
+  </si>
+  <si>
+    <t>18:41:03</t>
+  </si>
+  <si>
+    <t>05-20-2015</t>
+  </si>
+  <si>
+    <t>07:30:30</t>
+  </si>
+  <si>
+    <t>19:02:22</t>
+  </si>
+  <si>
+    <t>05-21-2015</t>
+  </si>
+  <si>
+    <t>06:56:26</t>
+  </si>
+  <si>
+    <t>18:50:16</t>
+  </si>
+  <si>
+    <t>05-22-2015</t>
+  </si>
+  <si>
+    <t>07:11:50</t>
+  </si>
+  <si>
+    <t>19:08:05</t>
   </si>
   <si>
     <t>NUMBER OF TIMES TARDY</t>
@@ -192,10 +201,13 @@
     <t>VL BALANCE</t>
   </si>
   <si>
+    <t>6.4.0</t>
+  </si>
+  <si>
+    <t>SL BALANCE</t>
+  </si>
+  <si>
     <t>7.4.0</t>
-  </si>
-  <si>
-    <t>SL BALANCE</t>
   </si>
   <si>
     <t>Employee has no time-in and therefore, considered as absent.</t>
@@ -619,799 +631,753 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="9" t="s">
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="P5" s="6" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="L5" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="M5" s="9" t="s">
+      <c r="B6" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="N5" s="9" t="s">
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6"/>
+      <c r="M6" s="6"/>
+      <c r="N6" s="6"/>
+      <c r="O6" s="6" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="P6" s="6" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="11"/>
+      <c r="N7" s="11"/>
+      <c r="O7" s="11" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="P7" s="11" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="11"/>
+      <c r="M8" s="11"/>
+      <c r="N8" s="11"/>
+      <c r="O8" s="11" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="P8" s="11" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="11"/>
+      <c r="M9" s="11"/>
+      <c r="N9" s="11"/>
+      <c r="O9" s="11" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="P9" s="11" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="11"/>
+      <c r="M10" s="11"/>
+      <c r="N10" s="11"/>
+      <c r="O10" s="11" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="P10" s="11" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="11"/>
+      <c r="M11" s="11"/>
+      <c r="N11" s="11"/>
+      <c r="O11" s="11" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="P11" s="11" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="6"/>
+      <c r="N12" s="6"/>
+      <c r="O12" s="6" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="P12" s="6" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="O5" s="9" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="P5" s="9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="9"/>
-      <c r="K6" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="L6" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="M6" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="N6" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="O6" s="9" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="P6" s="9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
-      <c r="J7" s="9"/>
-      <c r="K7" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="L7" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="M7" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="N7" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="O7" s="9" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="P7" s="9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="L8" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="M8" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="N8" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="O8" s="9" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="P8" s="9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="9"/>
-      <c r="K9" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="L9" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="M9" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="N9" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="O9" s="9" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="P9" s="9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="L10" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="M10" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="N10" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="O10" s="9" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="P10" s="9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="9"/>
-      <c r="K11" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="L11" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="M11" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="N11" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="O11" s="9" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="P11" s="9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
-      <c r="J12" s="9"/>
-      <c r="K12" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="L12" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="M12" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="N12" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="O12" s="9" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="P12" s="9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="9"/>
-      <c r="J13" s="9"/>
-      <c r="K13" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="L13" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="M13" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="N13" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="O13" s="9" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="P13" s="9" t="s">
-        <v>23</v>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="6"/>
+      <c r="M13" s="6"/>
+      <c r="N13" s="6"/>
+      <c r="O13" s="6" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="P13" s="6" t="inlineStr">
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="9" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C14" s="9"/>
       <c r="D14" s="9"/>
       <c r="E14" s="9"/>
       <c r="F14" s="9"/>
       <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
+      <c r="H14" s="9" t="n">
+        <v>1.0</v>
+      </c>
       <c r="I14" s="9"/>
       <c r="J14" s="9"/>
-      <c r="K14" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="L14" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="M14" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="N14" s="9" t="s">
-        <v>22</v>
-      </c>
+      <c r="K14" s="9"/>
+      <c r="L14" s="9"/>
+      <c r="M14" s="9"/>
+      <c r="N14" s="9"/>
       <c r="O14" s="9" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
       <c r="P14" s="9" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B15" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="9"/>
-      <c r="I15" s="9"/>
-      <c r="J15" s="9"/>
-      <c r="K15" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="L15" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="M15" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="N15" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="O15" s="9" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="P15" s="9" t="s">
-        <v>23</v>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="6"/>
+      <c r="M15" s="6"/>
+      <c r="N15" s="6"/>
+      <c r="O15" s="6" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="P15" s="6" t="inlineStr">
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="9" t="s">
+      <c r="A16" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B16" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="I16" s="9"/>
-      <c r="J16" s="9"/>
-      <c r="K16" s="9"/>
-      <c r="L16" s="9"/>
-      <c r="M16" s="9"/>
-      <c r="N16" s="9"/>
-      <c r="O16" s="9" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="P16" s="9" t="s">
+      <c r="B16" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="6" t="s">
         <v>41</v>
       </c>
+      <c r="D16" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="6"/>
+      <c r="M16" s="6"/>
+      <c r="N16" s="6"/>
+      <c r="O16" s="6" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="P16" s="6" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
     </row>
     <row r="17">
-      <c r="A17" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="B17" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="9"/>
-      <c r="J17" s="9"/>
-      <c r="K17" s="9"/>
-      <c r="L17" s="9"/>
-      <c r="M17" s="9"/>
-      <c r="N17" s="9"/>
-      <c r="O17" s="9" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="P17" s="9" t="s">
+      <c r="A17" s="6" t="s">
         <v>43</v>
       </c>
+      <c r="B17" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="6"/>
+      <c r="M17" s="6"/>
+      <c r="N17" s="6"/>
+      <c r="O17" s="6" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="P17" s="6" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
     </row>
     <row r="18">
-      <c r="A18" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="B18" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="9"/>
-      <c r="J18" s="9"/>
-      <c r="K18" s="9"/>
-      <c r="L18" s="9"/>
-      <c r="M18" s="9"/>
-      <c r="N18" s="9"/>
-      <c r="O18" s="9" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="P18" s="9" t="s">
-        <v>45</v>
+      <c r="A18" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="6"/>
+      <c r="M18" s="6"/>
+      <c r="N18" s="6"/>
+      <c r="O18" s="6" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="P18" s="6" t="inlineStr">
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="16" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B19" s="16" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C19" s="16" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="D19" s="16" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="E19" s="17" t="str">
-        <f>COUNT(E5:E15)</f>
+        <f>COUNT(E5:E18)</f>
       </c>
       <c r="F19" s="8" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="G19" s="8" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="H19" s="8" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="I19" s="8" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="J19" s="8" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="K19" s="8" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="L19" s="8" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="M19" s="8" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="N19" s="8" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="O19" s="8" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="P19" s="8" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="16" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C20" s="16" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="D20" s="16" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="E20" s="17" t="str">
-        <f>SUM(E5:E15)</f>
+        <f>SUM(E5:E18)</f>
       </c>
       <c r="F20" s="6" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="H20" s="6" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="I20" s="6" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="J20" s="6" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="K20" s="6" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="L20" s="6" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="M20" s="6" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="N20" s="6" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="O20" s="6" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="P20" s="6" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="16" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B21" s="16" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C21" s="16" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="D21" s="16" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="E21" s="16" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F21" s="16" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="G21" s="17" t="str">
         <f>SUM(G5:G18)</f>
       </c>
       <c r="H21" s="6" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="I21" s="6" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="J21" s="6" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="K21" s="6" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="L21" s="6" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="M21" s="6" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="N21" s="6" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="O21" s="6" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="P21" s="6" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="16" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C22" s="16" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="D22" s="16" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="E22" s="16" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F22" s="16" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="G22" s="16" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="H22" s="17" t="str">
-        <f>SUM(H5:H15)</f>
-      </c>
-      <c r="I22" s="6" t="str">
-        <f>SUM(I5:I15)</f>
+        <f>SUM(H5:H18)</f>
+      </c>
+      <c r="I22" s="17" t="str">
+        <f>SUM(I5:I18)</f>
       </c>
       <c r="J22" s="6" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="K22" s="6" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="L22" s="6" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="M22" s="6" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="N22" s="6" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="O22" s="6" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="P22" s="6" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="16" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B23" s="16" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C23" s="16" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="D23" s="16" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="E23" s="16" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F23" s="16" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="G23" s="16" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="H23" s="16" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="I23" s="17" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J23" s="6" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="K23" s="6" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="L23" s="6" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="M23" s="6" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="N23" s="6" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="O23" s="6" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="P23" s="6" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="7" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="H24" s="7" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="I24" s="7" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="J24" s="7" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="K24" s="7" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="L24" s="7" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="M24" s="7" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="N24" s="7" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="O24" s="7" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="P24" s="7" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="16" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B25" s="16" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C25" s="17" t="str">
         <f>FLOOR(G21/8,1)&amp;"."&amp;FLOOR(MOD(G21,8),1)&amp;"."&amp;(MOD(G21,8)-FLOOR(MOD(G21,8),1))*60</f>
       </c>
       <c r="D25" s="0" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="E25" s="0" t="inlineStr">
         <is>
@@ -1419,37 +1385,37 @@
         </is>
       </c>
       <c r="F25" s="0" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="I25" s="0" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="J25" s="0" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="K25" s="0" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="L25" s="0" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="M25" s="0" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="N25" s="0" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="O25" s="0" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="P25" s="0" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="Q25" s="0" t="str">
         <f>INT(LEFT(C26,2))</f>
@@ -1469,52 +1435,52 @@
     </row>
     <row r="26">
       <c r="A26" s="16" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B26" s="16" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C26" s="17" t="str">
         <f>FLOOR(I23,1)&amp;"."&amp;FLOOR(MOD(I23*8,8),1)&amp;"."&amp;(MOD(I23*8,8)-FLOOR(MOD(I23*8,8),1))*60</f>
       </c>
       <c r="D26" s="0" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="I26" s="4" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="K26" s="4" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="L26" s="4" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="M26" s="4" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="N26" s="4" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="O26" s="4" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="P26" s="4" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="Q26" s="0" t="str">
         <f>INT(LEFT(C27,2))</f>
@@ -1534,52 +1500,52 @@
     </row>
     <row r="27">
       <c r="A27" s="16" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B27" s="16" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C27" s="17" t="str">
         <f>FLOOR(E20/8,1)&amp;"."&amp;FLOOR(MOD(E20,8),1)&amp;"."&amp;(MOD(E20,8)-FLOOR(MOD(E20,8),1))*60</f>
       </c>
       <c r="D27" s="0" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="E27" s="12" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F27" s="15" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="G27" s="15" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="H27" s="15" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="I27" s="15" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="J27" s="15" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="K27" s="15" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="L27" s="15" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="M27" s="15" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="N27" s="15" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="O27" s="15" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="P27" s="15" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="Q27" s="0" t="str">
         <f>INT(LEFT(C28,2))</f>
@@ -1599,52 +1565,52 @@
     </row>
     <row r="28">
       <c r="A28" s="16" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B28" s="16" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C28" s="17" t="str">
         <f>FLOOR(H22,1)&amp;"."&amp;(H22-FLOOR(H22,1))*8&amp;".0"</f>
       </c>
       <c r="D28" s="0" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="E28" s="12" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F28" s="15" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="G28" s="15" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="H28" s="15" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="I28" s="15" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="J28" s="15" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="K28" s="15" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="L28" s="15" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="M28" s="15" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="N28" s="15" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="O28" s="15" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="P28" s="15" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="Q28" s="0" t="str">
         <f>INT(LEFT(C29,2))</f>
@@ -1664,52 +1630,52 @@
     </row>
     <row r="29">
       <c r="A29" s="16" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B29" s="16" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C29" s="17" t="str">
         <f>FLOOR(I22,1)&amp;"."&amp;(I22-FLOOR(I22,1))*8&amp;".0"</f>
       </c>
       <c r="D29" s="0" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="E29" s="13" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F29" s="15" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="G29" s="15" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="H29" s="15" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="I29" s="15" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="J29" s="15" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="K29" s="15" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="L29" s="15" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="M29" s="15" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="N29" s="15" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="O29" s="15" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="P29" s="15" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="Q29" s="0" t="str">
         <f>INT(LEFT(C30,2))</f>
@@ -1729,52 +1695,52 @@
     </row>
     <row r="30">
       <c r="A30" s="16" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B30" s="16" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C30" s="17" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="E30" s="13" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F30" s="15" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="G30" s="15" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="H30" s="15" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="I30" s="15" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="J30" s="15" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="K30" s="15" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="L30" s="15" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="M30" s="15" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="N30" s="15" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="O30" s="15" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="P30" s="15" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="Q30" s="0" t="str">
         <f>INT(LEFT(C31,2))</f>
@@ -1794,58 +1760,58 @@
     </row>
     <row r="31">
       <c r="A31" s="16" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B31" s="16" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C31" s="17" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="E31" s="14" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F31" s="15" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="G31" s="15" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="H31" s="15" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="I31" s="15" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="J31" s="15" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="K31" s="15" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="L31" s="15" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="M31" s="15" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="N31" s="15" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="O31" s="15" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="P31" s="15" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="Q31" s="0" t="str">
         <f>Q26+Q25+IF(Q27&gt;Q29,Q27-Q29,0)+IF(Q28&gt;Q30,Q28-Q30,0)</f>
       </c>
       <c r="R31" s="0" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="S31" s="0" t="str">
         <f>S26+S25+IF(S27&gt;S29,S27-S29,0)+IF(S28&gt;S30,S28-S30,0)</f>
@@ -1859,52 +1825,52 @@
     </row>
     <row r="32">
       <c r="A32" s="16" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="B32" s="16" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C32" s="17" t="str">
         <f>FLOOR(Q32/8,1)&amp;"."&amp;FLOOR(MOD(Q32,8),1)&amp;"."&amp;(MOD(Q32,8)-FLOOR(MOD(Q32,8),1))*60</f>
       </c>
       <c r="D32" s="0" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="E32" s="14" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F32" s="15" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="G32" s="15" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="H32" s="15" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="I32" s="15" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="J32" s="15" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="K32" s="15" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="L32" s="15" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="M32" s="15" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="N32" s="15" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="O32" s="15" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="P32" s="15" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="Q32" s="0" t="str">
         <f>U31/60</f>
@@ -1912,52 +1878,52 @@
     </row>
     <row r="33">
       <c r="A33" s="0" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="G33" s="7" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="H33" s="7" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="I33" s="7" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="J33" s="7" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="K33" s="7" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="L33" s="7" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="M33" s="7" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="N33" s="7" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="O33" s="7" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="P33" s="7" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>